<commit_message>
first attempt at understanding i2b2
</commit_message>
<xml_diff>
--- a/data/dddm_sample_data.xlsx
+++ b/data/dddm_sample_data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a6b9afb2ee4a130/Documents/All_of_Maras_R/DDDM/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_4BBFC2E4893369BC3E648C2CAB61E99F10F88B3C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3636989E-311C-4C31-B5F6-67BA6BA25F4B}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="23240" windowHeight="17000"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients with BCH MRNs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -198,9 +204,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yyyy\ h\:mm\:ss\ AM/PM"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h\:mm\:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -316,12 +323,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -331,15 +338,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -360,6 +377,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -684,31 +709,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" customWidth="1"/>
-    <col min="2" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="94.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="30.54296875" customWidth="1"/>
+    <col min="8" max="8" width="17.81640625" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="10" max="11" width="13.6328125" customWidth="1"/>
+    <col min="12" max="12" width="94.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="49" customHeight="1">
+    <row r="1" spans="1:12" ht="49" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -742,62 +771,64 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="13.5" customHeight="1">
+    <row r="2" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="1">
-        <v>37788496</v>
+      <c r="B2" s="7">
+        <v>37864379</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2">
         <v>42431.959837962961</v>
       </c>
-      <c r="E2" s="7">
-        <v>6065446.8820000002</v>
+      <c r="E2" s="8">
+        <v>6088564.6380000003</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2">
-        <v>42430</v>
+        <v>42418</v>
       </c>
       <c r="H2" s="2">
-        <v>42430.583333333343</v>
-      </c>
-      <c r="I2" s="2"/>
+        <v>42418.447916666657</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="J2" s="1">
-        <v>99204</v>
+        <v>99214</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="1">
-        <v>37788496</v>
+      <c r="B3" s="7">
+        <v>37864379</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2">
         <v>42431.959837962961</v>
       </c>
-      <c r="E3" s="7">
-        <v>6083938.3719999995</v>
+      <c r="E3" s="8">
+        <v>6076155.534</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2">
-        <v>42430</v>
+        <v>42431</v>
       </c>
       <c r="H3" s="2">
-        <v>42430.604166666657</v>
+        <v>42431.375</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>6</v>
@@ -806,25 +837,25 @@
         <v>99024</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="13.5" customHeight="1">
+    <row r="4" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="1">
-        <v>37792535</v>
+      <c r="B4" s="7">
+        <v>37864379</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2">
-        <v>42431.959826388891</v>
-      </c>
-      <c r="E4" s="7">
-        <v>2481789.9500000002</v>
+        <v>42431.959837962961</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6106495.892</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>5</v>
@@ -833,34 +864,34 @@
         <v>42431</v>
       </c>
       <c r="H4" s="2">
-        <v>42431.666666666657</v>
+        <v>42431.541666666657</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J4" s="1">
-        <v>99203</v>
+        <v>99244</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="13.5" customHeight="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="1">
-        <v>37792535</v>
+      <c r="B5" s="7">
+        <v>37804142</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2">
         <v>42431.959826388891</v>
       </c>
       <c r="E5" s="7">
-        <v>5173693.08</v>
+        <v>2542816.1859999998</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>5</v>
@@ -869,96 +900,96 @@
         <v>42431</v>
       </c>
       <c r="H5" s="2">
-        <v>42431.583333333343</v>
+        <v>42431.458333333343</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="1">
-        <v>99213</v>
+        <v>99242</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="13.5" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="1">
-        <v>37792535</v>
+      <c r="B6" s="7">
+        <v>37864379</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2">
-        <v>42431.959826388891</v>
-      </c>
-      <c r="E6" s="7">
-        <v>5310087.0999999996</v>
+        <v>42431.959837962961</v>
+      </c>
+      <c r="E6" s="8">
+        <v>6086011.4919999996</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G6" s="2">
         <v>42431</v>
       </c>
       <c r="H6" s="2">
-        <v>42431.458333333343</v>
+        <v>42431.416666666657</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J6" s="1">
-        <v>99024</v>
+        <v>99244</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="13.5" customHeight="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="1">
-        <v>37792535</v>
+      <c r="B7" s="7">
+        <v>37864379</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2">
-        <v>42431.959826388891</v>
-      </c>
-      <c r="E7" s="7">
-        <v>5484008.2939999998</v>
+        <v>42437.959837905095</v>
+      </c>
+      <c r="E7" s="8">
+        <v>6066643.8619999997</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2">
-        <v>42431</v>
+        <v>42404</v>
       </c>
       <c r="H7" s="2">
-        <v>42430.831250000003</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>6</v>
+        <v>42404.254861111112</v>
+      </c>
+      <c r="I7" s="2">
+        <v>42407.465277777781</v>
       </c>
       <c r="J7" s="1">
-        <v>99253</v>
+        <v>64786</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="1">
+      <c r="B8" s="7">
         <v>37792535</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -968,7 +999,7 @@
         <v>42431.959826388891</v>
       </c>
       <c r="E8" s="7">
-        <v>5686566.926</v>
+        <v>5310087.0999999996</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>5</v>
@@ -977,24 +1008,24 @@
         <v>42431</v>
       </c>
       <c r="H8" s="2">
-        <v>42431.625</v>
+        <v>42431.458333333343</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J8" s="1">
-        <v>99203</v>
+        <v>99024</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="13.5" customHeight="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="1">
+      <c r="B9" s="7">
         <v>37792535</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1004,33 +1035,33 @@
         <v>42431.959826388891</v>
       </c>
       <c r="E9" s="7">
-        <v>5687705.9079999998</v>
+        <v>2481789.9500000002</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G9" s="2">
         <v>42431</v>
       </c>
       <c r="H9" s="2">
-        <v>42431.479166666657</v>
+        <v>42431.666666666657</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J9" s="1">
-        <v>99213</v>
+        <v>99203</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="13.5" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="1">
+      <c r="B10" s="7">
         <v>37792535</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1040,295 +1071,295 @@
         <v>42431.959826388891</v>
       </c>
       <c r="E10" s="7">
-        <v>6050594.4579999996</v>
+        <v>5173693.08</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2">
         <v>42431</v>
       </c>
       <c r="H10" s="2">
-        <v>42431.541666666657</v>
+        <v>42431.583333333343</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J10" s="1">
-        <v>99203</v>
+        <v>99213</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="13.5" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="1">
-        <v>37804142</v>
+      <c r="B11" s="7">
+        <v>37792535</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2">
         <v>42431.959826388891</v>
       </c>
       <c r="E11" s="7">
-        <v>2542816.1859999998</v>
+        <v>6050594.4579999996</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2">
         <v>42431</v>
       </c>
       <c r="H11" s="2">
-        <v>42431.458333333343</v>
+        <v>42431.541666666657</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J11" s="1">
-        <v>99242</v>
+        <v>99203</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="13.5" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="1">
-        <v>37804142</v>
+      <c r="B12" s="7">
+        <v>37864379</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2">
-        <v>42431.959826388891</v>
-      </c>
-      <c r="E12" s="7">
-        <v>327441.90000000002</v>
+        <v>42437.959837905095</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5471931.1359999999</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="2">
-        <v>42431</v>
+        <v>42403</v>
       </c>
       <c r="H12" s="2">
-        <v>42431.4375</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>6</v>
+        <v>42403.539583333331</v>
+      </c>
+      <c r="I12" s="2">
+        <v>42418.520138888889</v>
       </c>
       <c r="J12" s="1">
-        <v>99214</v>
+        <v>13120</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="14.25" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="1">
-        <v>37804142</v>
+      <c r="B13" s="7">
+        <v>37864379</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2">
-        <v>42431.959826388891</v>
-      </c>
-      <c r="E13" s="7">
-        <v>5374894.3119999999</v>
+        <v>42437.959837905095</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5471931.1359999999</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G13" s="2">
-        <v>42431</v>
+        <v>42403</v>
       </c>
       <c r="H13" s="2">
-        <v>42431.416666666657</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>6</v>
+        <v>42403.539583333331</v>
+      </c>
+      <c r="I13" s="2">
+        <v>42418.520138888889</v>
       </c>
       <c r="J13" s="1">
-        <v>99213</v>
+        <v>61210</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="1">
-        <v>37804142</v>
+      <c r="B14" s="7">
+        <v>37864379</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2">
-        <v>42431.959826388891</v>
-      </c>
-      <c r="E14" s="7">
-        <v>5950166.602</v>
+        <v>42437.959837905095</v>
+      </c>
+      <c r="E14" s="8">
+        <v>5471931.1359999999</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="2">
-        <v>42431</v>
+        <v>42416</v>
       </c>
       <c r="H14" s="2">
-        <v>42431.375</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>6</v>
+        <v>42403.539583333331</v>
+      </c>
+      <c r="I14" s="2">
+        <v>42418.520138888889</v>
       </c>
       <c r="J14" s="1">
-        <v>99213</v>
+        <v>62223</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="13.5" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="1">
-        <v>37804142</v>
+      <c r="B15" s="7">
+        <v>37864379</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2">
-        <v>42431.959826388891</v>
-      </c>
-      <c r="E15" s="7">
-        <v>6013834.8319999995</v>
+        <v>42437.959837905095</v>
+      </c>
+      <c r="E15" s="8">
+        <v>5930815.0139999995</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G15" s="2">
-        <v>42431</v>
+        <v>42405</v>
       </c>
       <c r="H15" s="2">
-        <v>42431.395833333343</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>6</v>
+        <v>42405.282638888893</v>
+      </c>
+      <c r="I15" s="2">
+        <v>42407.558333333327</v>
       </c>
       <c r="J15" s="1">
-        <v>99213</v>
+        <v>62225</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="13.5" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="1">
-        <v>37804142</v>
+      <c r="B16" s="7">
+        <v>37864379</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2">
-        <v>42431.959837962961</v>
-      </c>
-      <c r="E16" s="7">
-        <v>6061016.8219999997</v>
+        <v>42437.959837905095</v>
+      </c>
+      <c r="E16" s="8">
+        <v>5930815.0139999995</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="2">
-        <v>42431</v>
+        <v>42405</v>
       </c>
       <c r="H16" s="2">
-        <v>42431.354166666657</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>6</v>
+        <v>42405.282638888893</v>
+      </c>
+      <c r="I16" s="2">
+        <v>42407.558333333327</v>
       </c>
       <c r="J16" s="1">
-        <v>99242</v>
+        <v>62230</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="13.5" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="1">
-        <v>37804142</v>
+      <c r="B17" s="7">
+        <v>37864379</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2">
-        <v>42431.959837962961</v>
-      </c>
-      <c r="E17" s="7">
-        <v>6090326.79</v>
+        <v>42437.959837905095</v>
+      </c>
+      <c r="E17" s="8">
+        <v>5471931.1359999999</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G17" s="2">
-        <v>42431</v>
+        <v>42403</v>
       </c>
       <c r="H17" s="2">
-        <v>42431.479166666657</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>6</v>
+        <v>42403.539583333331</v>
+      </c>
+      <c r="I17" s="2">
+        <v>42418.520138888889</v>
       </c>
       <c r="J17" s="1">
-        <v>99024</v>
+        <v>62256</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="1">
-        <v>37804142</v>
+      <c r="B18" s="7">
+        <v>37864379</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2">
-        <v>42431.959837962961</v>
-      </c>
-      <c r="E18" s="7">
-        <v>6104314.1799999997</v>
+        <v>42431.959826388891</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2746481.716</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>18</v>
@@ -1337,43 +1368,43 @@
         <v>42431</v>
       </c>
       <c r="H18" s="2">
-        <v>42431.520833333343</v>
+        <v>42431.458333333343</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J18" s="1">
-        <v>99242</v>
+        <v>99024</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="1">
-        <v>37804142</v>
+      <c r="B19" s="7">
+        <v>37864379</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>42431.959837962961</v>
       </c>
-      <c r="E19" s="7">
-        <v>6104999.0499999998</v>
+      <c r="E19" s="8">
+        <v>6093126.7359999996</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G19" s="2">
         <v>42431</v>
       </c>
       <c r="H19" s="2">
-        <v>42431.5</v>
+        <v>42431.395833333343</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>6</v>
@@ -1382,87 +1413,87 @@
         <v>99243</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="13.5" customHeight="1">
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="1">
-        <v>37804142</v>
+      <c r="B20" s="7">
+        <v>37792535</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D20" s="2">
-        <v>42431.959837962961</v>
+        <v>42431.959826388891</v>
       </c>
       <c r="E20" s="7">
-        <v>6108797.3020000001</v>
+        <v>5484008.2939999998</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G20" s="2">
         <v>42431</v>
       </c>
       <c r="H20" s="2">
-        <v>42431.541666666657</v>
+        <v>42430.831250000003</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J20" s="1">
-        <v>99242</v>
+        <v>99253</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="13.5" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="1">
-        <v>37820050</v>
+      <c r="B21" s="7">
+        <v>37792535</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D21" s="2">
-        <v>42432.959837905095</v>
+        <v>42431.959826388891</v>
       </c>
       <c r="E21" s="7">
-        <v>5064157.07</v>
+        <v>5687705.9079999998</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="2">
-        <v>42180</v>
+        <v>42431</v>
       </c>
       <c r="H21" s="2">
-        <v>42180.763888888891</v>
-      </c>
-      <c r="I21" s="2">
-        <v>42184.540972222218</v>
+        <v>42431.479166666657</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="J21" s="1">
-        <v>61210</v>
+        <v>99213</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="13.5" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="1">
+      <c r="B22" s="7">
         <v>37820050</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1471,34 +1502,34 @@
       <c r="D22" s="2">
         <v>42432.959837905095</v>
       </c>
-      <c r="E22" s="7">
-        <v>5064157.07</v>
+      <c r="E22" s="8">
+        <v>5636169.1320000002</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="2">
-        <v>42180</v>
+        <v>42183</v>
       </c>
       <c r="H22" s="2">
-        <v>42180.763888888891</v>
+        <v>42183.15625</v>
       </c>
       <c r="I22" s="2">
-        <v>42184.540972222218</v>
+        <v>42227.427777777782</v>
       </c>
       <c r="J22" s="1">
-        <v>62225</v>
+        <v>61313</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="14.25" customHeight="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="1">
+      <c r="B23" s="7">
         <v>37820050</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1507,7 +1538,7 @@
       <c r="D23" s="2">
         <v>42432.959837905095</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>5636169.1320000002</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1523,388 +1554,386 @@
         <v>42227.427777777782</v>
       </c>
       <c r="J23" s="1">
-        <v>61313</v>
+        <v>69990</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="13.5" customHeight="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="1">
-        <v>37820050</v>
+      <c r="B24" s="7">
+        <v>37788496</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2">
-        <v>42432.959837905095</v>
+        <v>42431.959837962961</v>
       </c>
       <c r="E24" s="7">
-        <v>5636169.1320000002</v>
+        <v>6083938.3719999995</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G24" s="2">
-        <v>42183</v>
+        <v>42430</v>
       </c>
       <c r="H24" s="2">
-        <v>42183.15625</v>
-      </c>
-      <c r="I24" s="2">
-        <v>42227.427777777782</v>
+        <v>42430.604166666657</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="J24" s="1">
-        <v>69990</v>
+        <v>99024</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="13.5" customHeight="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="1">
-        <v>37845088</v>
+      <c r="B25" s="7">
+        <v>37864379</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2">
-        <v>42436.959837905095</v>
-      </c>
-      <c r="E25" s="7">
-        <v>5732714.824</v>
+        <v>42431.959826388891</v>
+      </c>
+      <c r="E25" s="8">
+        <v>2539458.4720000001</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G25" s="2">
-        <v>42377</v>
+        <v>42418</v>
       </c>
       <c r="H25" s="2">
-        <v>42377.666666666657</v>
+        <v>42418.40625</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J25" s="1">
-        <v>99213</v>
+        <v>99243</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="13.5" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="1">
-        <v>37864379</v>
+      <c r="B26" s="7">
+        <v>37792535</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D26" s="2">
-        <v>42437.959837905095</v>
+        <v>42431.959826388891</v>
       </c>
       <c r="E26" s="7">
-        <v>5471931.1359999999</v>
+        <v>5686566.926</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G26" s="2">
-        <v>42403</v>
+        <v>42431</v>
       </c>
       <c r="H26" s="2">
-        <v>42403.539583333331</v>
-      </c>
-      <c r="I26" s="2">
-        <v>42418.520138888889</v>
+        <v>42431.625</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="J26" s="1">
-        <v>13120</v>
+        <v>99203</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="13.5" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="1">
-        <v>37864379</v>
+      <c r="B27" s="7">
+        <v>37788496</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D27" s="2">
-        <v>42437.959837905095</v>
+        <v>42431.959837962961</v>
       </c>
       <c r="E27" s="7">
-        <v>5471931.1359999999</v>
+        <v>6065446.8820000002</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G27" s="2">
-        <v>42403</v>
+        <v>42430</v>
       </c>
       <c r="H27" s="2">
-        <v>42403.539583333331</v>
-      </c>
-      <c r="I27" s="2">
-        <v>42418.520138888889</v>
-      </c>
+        <v>42430.583333333343</v>
+      </c>
+      <c r="I27" s="2"/>
       <c r="J27" s="1">
-        <v>61210</v>
+        <v>99204</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="14.25" customHeight="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="1">
-        <v>37864379</v>
+      <c r="B28" s="7">
+        <v>37804142</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D28" s="2">
-        <v>42437.959837905095</v>
+        <v>42431.959826388891</v>
       </c>
       <c r="E28" s="7">
-        <v>5471931.1359999999</v>
+        <v>327441.90000000002</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G28" s="2">
-        <v>42403</v>
+        <v>42431</v>
       </c>
       <c r="H28" s="2">
-        <v>42403.539583333331</v>
-      </c>
-      <c r="I28" s="2">
-        <v>42418.520138888889</v>
+        <v>42431.4375</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="J28" s="1">
-        <v>62256</v>
+        <v>99214</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="13.5" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="1">
-        <v>37864379</v>
+      <c r="B29" s="7">
+        <v>37804142</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D29" s="2">
-        <v>42437.959837905095</v>
-      </c>
-      <c r="E29" s="7">
-        <v>5471931.1359999999</v>
+        <v>42431.959837962961</v>
+      </c>
+      <c r="E29" s="8">
+        <v>6061016.8219999997</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G29" s="2">
-        <v>42416</v>
+        <v>42431</v>
       </c>
       <c r="H29" s="2">
-        <v>42403.539583333331</v>
-      </c>
-      <c r="I29" s="2">
-        <v>42418.520138888889</v>
+        <v>42431.354166666657</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="J29" s="1">
-        <v>62223</v>
+        <v>99242</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="13.5" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="1">
-        <v>37864379</v>
+      <c r="B30" s="7">
+        <v>37804142</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D30" s="2">
-        <v>42437.959837905095</v>
-      </c>
-      <c r="E30" s="7">
-        <v>5930815.0139999995</v>
+        <v>42431.959837962961</v>
+      </c>
+      <c r="E30" s="8">
+        <v>6090326.79</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G30" s="2">
-        <v>42405</v>
+        <v>42431</v>
       </c>
       <c r="H30" s="2">
-        <v>42405.282638888893</v>
-      </c>
-      <c r="I30" s="2">
-        <v>42407.558333333327</v>
+        <v>42431.479166666657</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="J30" s="1">
-        <v>62225</v>
+        <v>99024</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="13.5" customHeight="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="1">
-        <v>37864379</v>
+      <c r="B31" s="7">
+        <v>37804142</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D31" s="2">
-        <v>42437.959837905095</v>
-      </c>
-      <c r="E31" s="7">
-        <v>5930815.0139999995</v>
+        <v>42431.959826388891</v>
+      </c>
+      <c r="E31" s="8">
+        <v>5374894.3119999999</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G31" s="2">
-        <v>42405</v>
+        <v>42431</v>
       </c>
       <c r="H31" s="2">
-        <v>42405.282638888893</v>
-      </c>
-      <c r="I31" s="2">
-        <v>42407.558333333327</v>
+        <v>42431.416666666657</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="J31" s="1">
-        <v>62230</v>
+        <v>99213</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="13.5" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="1">
-        <v>37864379</v>
+      <c r="B32" s="7">
+        <v>37804142</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D32" s="2">
-        <v>42437.959837905095</v>
-      </c>
-      <c r="E32" s="7">
-        <v>6066643.8619999997</v>
+        <v>42431.959826388891</v>
+      </c>
+      <c r="E32" s="8">
+        <v>5950166.602</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G32" s="2">
-        <v>42404</v>
+        <v>42431</v>
       </c>
       <c r="H32" s="2">
-        <v>42404.254861111112</v>
-      </c>
-      <c r="I32" s="2">
-        <v>42407.465277777781</v>
+        <v>42431.375</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="J32" s="1">
-        <v>64786</v>
+        <v>99213</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="14.25" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="1">
-        <v>37864379</v>
+      <c r="B33" s="7">
+        <v>37804142</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D33" s="2">
         <v>42431.959826388891</v>
       </c>
-      <c r="E33" s="7">
-        <v>2539458.4720000001</v>
+      <c r="E33" s="8">
+        <v>6013834.8319999995</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G33" s="2">
-        <v>42418</v>
+        <v>42431</v>
       </c>
       <c r="H33" s="2">
-        <v>42418.40625</v>
+        <v>42431.395833333343</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J33" s="1">
-        <v>99243</v>
+        <v>99213</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="13.5" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="1">
-        <v>37864379</v>
+      <c r="B34" s="7">
+        <v>37804142</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D34" s="2">
-        <v>42431.959826388891</v>
-      </c>
-      <c r="E34" s="7">
-        <v>2746481.716</v>
+        <v>42431.959837962961</v>
+      </c>
+      <c r="E34" s="8">
+        <v>6108797.3020000001</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>18</v>
@@ -1913,70 +1942,70 @@
         <v>42431</v>
       </c>
       <c r="H34" s="2">
-        <v>42431.458333333343</v>
+        <v>42431.541666666657</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J34" s="1">
-        <v>99024</v>
+        <v>99242</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="13.5" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="1">
-        <v>37864379</v>
+      <c r="B35" s="7">
+        <v>37804142</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D35" s="2">
         <v>42431.959837962961</v>
       </c>
-      <c r="E35" s="7">
-        <v>6076155.534</v>
+      <c r="E35" s="8">
+        <v>6104999.0499999998</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G35" s="2">
         <v>42431</v>
       </c>
       <c r="H35" s="2">
-        <v>42431.375</v>
+        <v>42431.5</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J35" s="1">
-        <v>99024</v>
+        <v>99243</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="13.5" customHeight="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="1">
-        <v>37864379</v>
+      <c r="B36" s="7">
+        <v>37804142</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D36" s="2">
         <v>42431.959837962961</v>
       </c>
-      <c r="E36" s="7">
-        <v>6086011.4919999996</v>
+      <c r="E36" s="8">
+        <v>6104314.1799999997</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>18</v>
@@ -1985,132 +2014,135 @@
         <v>42431</v>
       </c>
       <c r="H36" s="2">
-        <v>42431.416666666657</v>
+        <v>42431.520833333343</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J36" s="1">
-        <v>99244</v>
+        <v>99242</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="13.5" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="1">
-        <v>37864379</v>
+      <c r="B37" s="7">
+        <v>37845088</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D37" s="2">
-        <v>42431.959837962961</v>
-      </c>
-      <c r="E37" s="7">
-        <v>6088564.6380000003</v>
+        <v>42436.959837905095</v>
+      </c>
+      <c r="E37" s="8">
+        <v>5732714.824</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="2">
+        <v>42377</v>
+      </c>
+      <c r="H37" s="2">
+        <v>42377.666666666657</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="1">
+        <v>99213</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="7">
+        <v>37820050</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="2">
+        <v>42432.959837905095</v>
+      </c>
+      <c r="E38" s="8">
+        <v>5064157.07</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="2">
-        <v>42418</v>
-      </c>
-      <c r="H37" s="2">
-        <v>42418.447916666657</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J37" s="1">
-        <v>99214</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="1">
-        <v>37864379</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="2">
-        <v>42431.959837962961</v>
-      </c>
-      <c r="E38" s="7">
-        <v>6093126.7359999996</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G38" s="2">
-        <v>42431</v>
+        <v>42180</v>
       </c>
       <c r="H38" s="2">
-        <v>42431.395833333343</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>6</v>
+        <v>42180.763888888891</v>
+      </c>
+      <c r="I38" s="2">
+        <v>42184.540972222218</v>
       </c>
       <c r="J38" s="1">
-        <v>99243</v>
+        <v>61210</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="13.5" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" s="5">
-        <v>37864379</v>
+      <c r="B39" s="11">
+        <v>37820050</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D39" s="6">
-        <v>42431.959837962961</v>
-      </c>
-      <c r="E39" s="8">
-        <v>6106495.892</v>
+        <v>42432.959837905095</v>
+      </c>
+      <c r="E39" s="9">
+        <v>5064157.07</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G39" s="6">
-        <v>42431</v>
+        <v>42180</v>
       </c>
       <c r="H39" s="6">
-        <v>42431.541666666657</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>6</v>
+        <v>42180.763888888891</v>
+      </c>
+      <c r="I39" s="6">
+        <v>42184.540972222218</v>
       </c>
       <c r="J39" s="5">
-        <v>99244</v>
+        <v>62225</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="L39" s="5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L39">
+    <sortCondition ref="K1:K39"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>